<commit_message>
include Jaguar I-Pace example
</commit_message>
<xml_diff>
--- a/example notebooks/case study publication BatPaC V5/data/ODYM_database/3_PR_material_price_mass_v1.xlsx
+++ b/example notebooks/case study publication BatPaC V5/data/ODYM_database/3_PR_material_price_mass_v1.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="121" documentId="13_ncr:1_{9126A6F2-D5E0-4780-B380-C6AB62921918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DCB7221C-57A7-4475-85E4-7F4D632D062B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E070B693-B126-4C45-8900-01C018EA8DC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10272" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -13,9 +13,10 @@
     <sheet name="Sheet2" sheetId="11" r:id="rId3"/>
     <sheet name="Literature" sheetId="5" r:id="rId4"/>
     <sheet name="Separator" sheetId="6" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId6"/>
+    <externalReference r:id="rId7"/>
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$D$1</definedName>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="246">
   <si>
     <t>Date created</t>
   </si>
@@ -604,9 +605,6 @@
     <t>ODYM Parameter File</t>
   </si>
   <si>
-    <t>cathode active material (NMC532/50%/LMO  - )</t>
-  </si>
-  <si>
     <t>density</t>
   </si>
   <si>
@@ -727,9 +725,6 @@
     <t>module electronics</t>
   </si>
   <si>
-    <t>module interconnect panels</t>
-  </si>
-  <si>
     <t>module row rack</t>
   </si>
   <si>
@@ -754,18 +749,9 @@
     <t>pack terminals</t>
   </si>
   <si>
-    <t>battery jacket aluminium</t>
-  </si>
-  <si>
-    <t>battery jacket steel</t>
-  </si>
-  <si>
     <t>battery jacket insulation</t>
   </si>
   <si>
-    <t>STILL CONVERT FROM M2 TO KG</t>
-  </si>
-  <si>
     <t>busbar</t>
   </si>
   <si>
@@ -773,6 +759,24 @@
   </si>
   <si>
     <t>Only unit prices</t>
+  </si>
+  <si>
+    <t>battery jacket Al</t>
+  </si>
+  <si>
+    <t>battery jacket Fe</t>
+  </si>
+  <si>
+    <t>cathode active material (50%/50% NMC532/LMO - )</t>
+  </si>
+  <si>
+    <t>module polymer panels</t>
+  </si>
+  <si>
+    <t>pack heater</t>
+  </si>
+  <si>
+    <t>Calculated from m2 (3 $/m2) based on a density of 0.32 g/cm3 as stated in BatPaC</t>
   </si>
 </sst>
 </file>
@@ -1579,21 +1583,21 @@
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.68359375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" customWidth="1"/>
-    <col min="3" max="3" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.41796875" customWidth="1"/>
-    <col min="5" max="5" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="30.41796875" customWidth="1"/>
-    <col min="7" max="7" width="6.578125" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" customWidth="1"/>
     <col min="8" max="8" width="43" customWidth="1"/>
-    <col min="9" max="9" width="3.41796875" customWidth="1"/>
-    <col min="10" max="11" width="3.26171875" customWidth="1"/>
+    <col min="9" max="9" width="3.42578125" customWidth="1"/>
+    <col min="10" max="11" width="3.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>187</v>
       </c>
@@ -1602,7 +1606,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
@@ -1615,7 +1619,7 @@
       </c>
       <c r="L2" s="1"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>4</v>
       </c>
@@ -1628,7 +1632,7 @@
       </c>
       <c r="L3" s="1"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>5</v>
       </c>
@@ -1641,7 +1645,7 @@
       </c>
       <c r="L4" s="1"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
@@ -1654,7 +1658,7 @@
       </c>
       <c r="L5" s="1"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>26</v>
       </c>
@@ -1670,7 +1674,7 @@
       </c>
       <c r="L6" s="1"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>27</v>
       </c>
@@ -1683,7 +1687,7 @@
       </c>
       <c r="L7" s="1"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>7</v>
       </c>
@@ -1696,7 +1700,7 @@
       </c>
       <c r="L8" s="1"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1707,7 +1711,7 @@
       </c>
       <c r="L9" s="1"/>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1717,7 +1721,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>0</v>
       </c>
@@ -1730,7 +1734,7 @@
       </c>
       <c r="L11" s="1"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>1</v>
       </c>
@@ -1743,7 +1747,7 @@
       </c>
       <c r="L12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -1756,7 +1760,7 @@
       </c>
       <c r="L13" s="1"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>10</v>
       </c>
@@ -1769,7 +1773,7 @@
       </c>
       <c r="L14" s="1"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>11</v>
       </c>
@@ -1782,7 +1786,7 @@
       </c>
       <c r="L15" s="1"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
         <v>39</v>
       </c>
@@ -1791,7 +1795,7 @@
       <c r="E16" s="1"/>
       <c r="L16" s="1"/>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>39</v>
       </c>
@@ -1800,7 +1804,7 @@
       <c r="E17" s="1"/>
       <c r="L17" s="1"/>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>39</v>
       </c>
@@ -1809,7 +1813,7 @@
       <c r="E18" s="1"/>
       <c r="L18" s="1"/>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>39</v>
       </c>
@@ -1818,7 +1822,7 @@
       <c r="E19" s="1"/>
       <c r="L19" s="1"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>39</v>
       </c>
@@ -1828,7 +1832,7 @@
       <c r="F20" s="1"/>
       <c r="L20" s="1"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
         <v>12</v>
       </c>
@@ -1848,7 +1852,7 @@
       </c>
       <c r="L21" s="1"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
         <v>176</v>
       </c>
@@ -1867,7 +1871,7 @@
       <c r="H22" s="9"/>
       <c r="L22" s="1"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="16" t="s">
         <v>185</v>
       </c>
@@ -1890,7 +1894,7 @@
       </c>
       <c r="L23" s="1"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="16"/>
       <c r="B24" s="35"/>
       <c r="C24" s="16" t="s">
@@ -1909,7 +1913,7 @@
       </c>
       <c r="L24" s="1"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="35"/>
       <c r="B25" s="35"/>
       <c r="C25" s="16" t="s">
@@ -1926,7 +1930,7 @@
       </c>
       <c r="L25" s="1"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="35"/>
       <c r="B26" s="35"/>
       <c r="C26" s="16" t="s">
@@ -1943,7 +1947,7 @@
       </c>
       <c r="L26" s="1"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="G27" s="21" t="s">
         <v>23</v>
       </c>
@@ -1953,7 +1957,7 @@
       <c r="K27" s="12"/>
       <c r="L27" s="13"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E28" s="1"/>
       <c r="F28" s="12"/>
       <c r="H28" s="12"/>
@@ -1962,35 +1966,35 @@
       <c r="K28" s="12"/>
       <c r="L28" s="13"/>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H29" s="12"/>
       <c r="I29" s="12"/>
       <c r="J29" s="12"/>
       <c r="K29" s="12"/>
       <c r="L29" s="12"/>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H30" s="12"/>
       <c r="I30" s="12"/>
       <c r="J30" s="12"/>
       <c r="K30" s="12"/>
       <c r="L30" s="12"/>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H31" s="12"/>
       <c r="I31" s="12"/>
       <c r="J31" s="12"/>
       <c r="K31" s="12"/>
       <c r="L31" s="12"/>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H32" s="11"/>
       <c r="I32" s="11"/>
       <c r="J32" s="12"/>
       <c r="K32" s="12"/>
       <c r="L32" s="12"/>
     </row>
-    <row r="33" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G33" s="12"/>
       <c r="H33" s="12"/>
       <c r="I33" s="12"/>
@@ -1998,7 +2002,7 @@
       <c r="K33" s="12"/>
       <c r="L33" s="12"/>
     </row>
-    <row r="34" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="5:12" x14ac:dyDescent="0.25">
       <c r="G34" s="12"/>
       <c r="H34" s="12"/>
       <c r="I34" s="12"/>
@@ -2006,7 +2010,7 @@
       <c r="K34" s="12"/>
       <c r="L34" s="12"/>
     </row>
-    <row r="35" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E35" s="12"/>
       <c r="F35" s="12"/>
       <c r="G35" s="12"/>
@@ -2016,7 +2020,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="5:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="5:12" x14ac:dyDescent="0.25">
       <c r="E36" s="12"/>
       <c r="F36" s="12"/>
       <c r="G36" s="12"/>
@@ -2036,26 +2040,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8BDDE9FA-34B5-487F-BD06-B5E05371CD58}">
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B58" sqref="B58"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="A65:B68"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="58.26171875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.26171875" style="40" customWidth="1"/>
-    <col min="3" max="3" width="6.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="81.15625" customWidth="1"/>
+    <col min="1" max="1" width="58.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="40" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.140625" customWidth="1"/>
     <col min="5" max="5" width="80" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="28.68359375" customWidth="1"/>
-    <col min="8" max="8" width="32.578125" customWidth="1"/>
-    <col min="9" max="9" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.7109375" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.6" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>185</v>
       </c>
@@ -2080,7 +2084,7 @@
       <c r="N1" s="36"/>
       <c r="O1" s="36"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="35" t="s">
         <v>139</v>
       </c>
@@ -2091,10 +2095,10 @@
         <v>93</v>
       </c>
       <c r="D2" s="35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="35" t="s">
         <v>140</v>
       </c>
@@ -2105,10 +2109,10 @@
         <v>93</v>
       </c>
       <c r="D3" s="35" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
         <v>141</v>
       </c>
@@ -2122,7 +2126,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="35" t="s">
         <v>142</v>
       </c>
@@ -2133,10 +2137,10 @@
         <v>93</v>
       </c>
       <c r="D5" s="35" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="35" t="s">
         <v>143</v>
       </c>
@@ -2147,10 +2151,10 @@
         <v>93</v>
       </c>
       <c r="D6" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
         <v>144</v>
       </c>
@@ -2161,10 +2165,10 @@
         <v>93</v>
       </c>
       <c r="D7" s="35" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="35" t="s">
         <v>145</v>
       </c>
@@ -2175,11 +2179,11 @@
         <v>93</v>
       </c>
       <c r="D8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E8" s="35"/>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="35" t="s">
         <v>146</v>
       </c>
@@ -2190,11 +2194,11 @@
         <v>93</v>
       </c>
       <c r="D9" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E9" s="35"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="35" t="s">
         <v>147</v>
       </c>
@@ -2205,11 +2209,11 @@
         <v>93</v>
       </c>
       <c r="D10" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E10" s="35"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="35" t="s">
         <v>148</v>
       </c>
@@ -2220,13 +2224,13 @@
         <v>93</v>
       </c>
       <c r="D11" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E11" s="35"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="35" t="s">
-        <v>188</v>
+        <v>242</v>
       </c>
       <c r="B12" s="39">
         <v>24.47635</v>
@@ -2235,11 +2239,11 @@
         <v>93</v>
       </c>
       <c r="D12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E12" s="35"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="35" t="s">
         <v>149</v>
       </c>
@@ -2250,11 +2254,11 @@
         <v>93</v>
       </c>
       <c r="D13" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E13" s="35"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="35" t="s">
         <v>131</v>
       </c>
@@ -2269,7 +2273,7 @@
       </c>
       <c r="E14" s="35"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="35" t="s">
         <v>164</v>
       </c>
@@ -2284,7 +2288,7 @@
       </c>
       <c r="E15" s="35"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="35" t="s">
         <v>150</v>
       </c>
@@ -2295,13 +2299,13 @@
         <v>93</v>
       </c>
       <c r="D16" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="38" t="s">
         <v>151</v>
       </c>
@@ -2312,13 +2316,13 @@
         <v>93</v>
       </c>
       <c r="D17" s="35" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E17" s="35" t="s">
-        <v>225</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="38" t="s">
         <v>152</v>
       </c>
@@ -2329,11 +2333,11 @@
         <v>93</v>
       </c>
       <c r="D18" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E18" s="35"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="38" t="s">
         <v>165</v>
       </c>
@@ -2348,9 +2352,9 @@
       </c>
       <c r="E19" s="35"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B20" s="39">
         <v>2.9</v>
@@ -2359,13 +2363,13 @@
         <v>93</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E20" s="35"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="35" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B21" s="39">
         <v>2.9</v>
@@ -2374,11 +2378,11 @@
         <v>93</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E21" s="35"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="35" t="s">
         <v>153</v>
       </c>
@@ -2389,11 +2393,11 @@
         <v>93</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E22" s="35"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="35" t="s">
         <v>154</v>
       </c>
@@ -2404,13 +2408,13 @@
         <v>93</v>
       </c>
       <c r="D23" s="35" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E23" s="35"/>
     </row>
-    <row r="24" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="35" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B24" s="39">
         <v>2.746</v>
@@ -2419,10 +2423,10 @@
         <v>93</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="35" t="s">
         <v>155</v>
       </c>
@@ -2433,12 +2437,12 @@
         <v>93</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="35" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B26" s="40">
         <v>2.4321000000000002</v>
@@ -2447,12 +2451,12 @@
         <v>93</v>
       </c>
       <c r="D26" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="35" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B27" s="40">
         <v>2.4321000000000002</v>
@@ -2461,12 +2465,12 @@
         <v>93</v>
       </c>
       <c r="D27" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B28" s="40">
         <v>2.4321000000000002</v>
@@ -2475,10 +2479,10 @@
         <v>93</v>
       </c>
       <c r="D28" s="35" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="35" t="s">
         <v>133</v>
       </c>
@@ -2489,12 +2493,12 @@
         <v>93</v>
       </c>
       <c r="D29" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="35" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B30" s="39">
         <v>17.002960000000002</v>
@@ -2503,10 +2507,10 @@
         <v>93</v>
       </c>
       <c r="D30" s="35" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="35" t="s">
         <v>134</v>
       </c>
@@ -2517,12 +2521,12 @@
         <v>93</v>
       </c>
       <c r="D31" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B32" s="39">
         <v>15.43505</v>
@@ -2531,12 +2535,12 @@
         <v>93</v>
       </c>
       <c r="D32" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="35" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B33" s="39">
         <v>15.43505</v>
@@ -2545,12 +2549,12 @@
         <v>93</v>
       </c>
       <c r="D33" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="35" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B34" s="39">
         <v>15.43505</v>
@@ -2559,12 +2563,12 @@
         <v>93</v>
       </c>
       <c r="D34" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="35" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B35" s="39">
         <v>15.43505</v>
@@ -2573,12 +2577,12 @@
         <v>93</v>
       </c>
       <c r="D35" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B36" s="39">
         <v>15.43505</v>
@@ -2587,12 +2591,12 @@
         <v>93</v>
       </c>
       <c r="D36" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="35" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B37" s="39">
         <v>15.43505</v>
@@ -2601,10 +2605,10 @@
         <v>93</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>135</v>
       </c>
@@ -2615,10 +2619,10 @@
         <v>93</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="35" t="s">
         <v>136</v>
       </c>
@@ -2629,10 +2633,10 @@
         <v>93</v>
       </c>
       <c r="D39" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="35" t="s">
         <v>137</v>
       </c>
@@ -2643,10 +2647,10 @@
         <v>93</v>
       </c>
       <c r="D40" s="35" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="35" t="s">
         <v>124</v>
       </c>
@@ -2657,13 +2661,13 @@
         <v>93</v>
       </c>
       <c r="D41" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E41" s="35" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="42" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="35" t="s">
         <v>125</v>
       </c>
@@ -2674,13 +2678,13 @@
         <v>93</v>
       </c>
       <c r="D42" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E42" s="35" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="43" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="35" t="s">
         <v>126</v>
       </c>
@@ -2691,13 +2695,13 @@
         <v>93</v>
       </c>
       <c r="D43" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E43" s="35" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="44" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="35" t="s">
         <v>127</v>
       </c>
@@ -2708,13 +2712,13 @@
         <v>93</v>
       </c>
       <c r="D44" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E44" s="35" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="45" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="35" t="s">
         <v>128</v>
       </c>
@@ -2725,13 +2729,13 @@
         <v>93</v>
       </c>
       <c r="D45" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E45" s="35" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="46" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="35" t="s">
         <v>129</v>
       </c>
@@ -2742,13 +2746,13 @@
         <v>93</v>
       </c>
       <c r="D46" s="35" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E46" s="35" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="47" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="35" t="s">
         <v>156</v>
       </c>
@@ -2759,10 +2763,10 @@
         <v>93</v>
       </c>
       <c r="D47" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="35" t="s">
         <v>138</v>
       </c>
@@ -2773,11 +2777,11 @@
         <v>93</v>
       </c>
       <c r="D48" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E48" s="35"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="35" t="s">
         <v>166</v>
       </c>
@@ -2788,13 +2792,13 @@
         <v>93</v>
       </c>
       <c r="D49" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="E49" s="35"/>
+    </row>
+    <row r="50" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="35" t="s">
         <v>227</v>
-      </c>
-      <c r="E49" s="35"/>
-    </row>
-    <row r="50" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A50" s="35" t="s">
-        <v>228</v>
       </c>
       <c r="B50" s="39">
         <v>0</v>
@@ -2803,13 +2807,13 @@
         <v>93</v>
       </c>
       <c r="D50" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E50" s="35" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="35" t="s">
         <v>160</v>
       </c>
@@ -2820,12 +2824,12 @@
         <v>93</v>
       </c>
       <c r="D51" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="35" t="s">
-        <v>229</v>
+        <v>243</v>
       </c>
       <c r="B52" s="39">
         <v>2.2999999999999998</v>
@@ -2834,10 +2838,10 @@
         <v>93</v>
       </c>
       <c r="D52" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="35" t="s">
         <v>158</v>
       </c>
@@ -2848,10 +2852,10 @@
         <v>93</v>
       </c>
       <c r="D53" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="35" t="s">
         <v>157</v>
       </c>
@@ -2862,12 +2866,12 @@
         <v>93</v>
       </c>
       <c r="D54" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="35" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B55" s="35">
         <v>1.33</v>
@@ -2876,12 +2880,12 @@
         <v>93</v>
       </c>
       <c r="D55" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="35" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B56" s="35">
         <v>1</v>
@@ -2890,10 +2894,10 @@
         <v>93</v>
       </c>
       <c r="D56" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="35" t="s">
         <v>159</v>
       </c>
@@ -2904,13 +2908,13 @@
         <v>93</v>
       </c>
       <c r="D57" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E57" s="35" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="35" t="s">
         <v>161</v>
       </c>
@@ -2921,13 +2925,13 @@
         <v>93</v>
       </c>
       <c r="D58" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E58" s="35"/>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="35" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B59" s="35">
         <v>2.8</v>
@@ -2936,12 +2940,12 @@
         <v>93</v>
       </c>
       <c r="D59" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="60" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="35" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B60" s="35">
         <v>8</v>
@@ -2950,15 +2954,15 @@
         <v>93</v>
       </c>
       <c r="D60" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E60" s="35" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="61" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="35" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B61" s="35">
         <v>8</v>
@@ -2967,15 +2971,15 @@
         <v>93</v>
       </c>
       <c r="D61" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E61" s="35" t="s">
-        <v>236</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="35" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B62" s="35">
         <v>8.8800000000000008</v>
@@ -2984,12 +2988,12 @@
         <v>93</v>
       </c>
       <c r="D62" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="35" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="B63" s="35">
         <v>1.4</v>
@@ -2998,12 +3002,12 @@
         <v>93</v>
       </c>
       <c r="D63" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="35" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="B64" s="35">
         <v>2.81</v>
@@ -3012,26 +3016,29 @@
         <v>93</v>
       </c>
       <c r="D64" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="35" t="s">
-        <v>240</v>
-      </c>
-      <c r="B65" s="33" t="s">
-        <v>241</v>
+        <v>236</v>
+      </c>
+      <c r="B65" s="35">
+        <v>9.375</v>
       </c>
       <c r="C65" s="41" t="s">
         <v>93</v>
       </c>
       <c r="D65" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+      <c r="E65" s="35" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="35" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="B66" s="35">
         <v>8.68</v>
@@ -3040,12 +3047,12 @@
         <v>93</v>
       </c>
       <c r="D66" s="35" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="67" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="35" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="B67" s="35">
         <v>0</v>
@@ -3054,112 +3061,125 @@
         <v>93</v>
       </c>
       <c r="D67" s="35" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E67" s="35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="51" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A68" s="51"/>
-    </row>
-    <row r="69" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A69" s="51"/>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B68" s="35">
+        <v>0</v>
+      </c>
+      <c r="C68" s="41" t="s">
+        <v>93</v>
+      </c>
+      <c r="D68" s="35" t="s">
+        <v>226</v>
+      </c>
+      <c r="E68" s="35" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" s="35" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="35"/>
       <c r="B70" s="35"/>
       <c r="C70" s="35"/>
       <c r="D70" s="35"/>
       <c r="E70" s="35"/>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="35"/>
       <c r="B71" s="35"/>
       <c r="C71" s="35"/>
       <c r="D71" s="35"/>
       <c r="E71" s="35"/>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A72" s="35"/>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="35"/>
       <c r="C72" s="35"/>
       <c r="D72" s="35"/>
       <c r="E72" s="35"/>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="35"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="35"/>
       <c r="B74" s="35"/>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="35"/>
       <c r="B75" s="35"/>
       <c r="C75" s="35"/>
       <c r="D75" s="35"/>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="35"/>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B76" s="35"/>
       <c r="C76" s="35"/>
       <c r="D76" s="35"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B77" s="35"/>
       <c r="C77" s="35"/>
       <c r="D77" s="35"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B78" s="35"/>
       <c r="C78" s="35"/>
       <c r="D78" s="35"/>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B79" s="35"/>
       <c r="C79" s="35"/>
       <c r="D79" s="35"/>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A80" s="35"/>
       <c r="B80" s="35"/>
       <c r="C80" s="35"/>
       <c r="D80" s="35"/>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="35"/>
       <c r="B81" s="35"/>
       <c r="D81" s="35"/>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="35"/>
       <c r="B82" s="35"/>
       <c r="C82" s="35"/>
       <c r="D82" s="35"/>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="35"/>
       <c r="B83" s="35"/>
       <c r="C83" s="35"/>
       <c r="D83" s="35"/>
     </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="35"/>
       <c r="B84" s="35"/>
       <c r="C84" s="35"/>
       <c r="D84" s="35"/>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="35"/>
       <c r="B85" s="35"/>
       <c r="C85" s="35"/>
       <c r="D85" s="35"/>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="35"/>
       <c r="B86" s="35"/>
       <c r="C86" s="35"/>
       <c r="D86" s="35"/>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A87" s="35"/>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B87" s="35"/>
       <c r="C87" s="35"/>
       <c r="D87" s="35"/>
@@ -3179,237 +3199,237 @@
       <selection activeCell="D56" sqref="A1:D56"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.83984375" style="35" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.41796875" style="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.41796875" style="35" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" style="35" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.42578125" style="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="35" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="27" style="35" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="9.15625" style="35"/>
+    <col min="5" max="16384" width="9.140625" style="35"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2"/>
       <c r="B1" s="42"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B2" s="39"/>
       <c r="C2" s="41"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="38"/>
       <c r="B3" s="39"/>
       <c r="C3" s="41"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="38"/>
       <c r="B4" s="39"/>
       <c r="C4" s="41"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="38"/>
       <c r="B5" s="39"/>
       <c r="C5" s="41"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B6" s="39"/>
       <c r="C6" s="41"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="39"/>
       <c r="C7" s="41"/>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="39"/>
       <c r="C8" s="41"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="39"/>
       <c r="C9" s="41"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="39"/>
       <c r="C10" s="41"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="39"/>
       <c r="C11" s="41"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="39"/>
       <c r="C12" s="41"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="39"/>
       <c r="C13" s="41"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="39"/>
       <c r="C14" s="41"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="39"/>
       <c r="C15" s="41"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="39"/>
       <c r="C16" s="41"/>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B18" s="39"/>
       <c r="C18" s="41"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B19" s="39"/>
       <c r="C19" s="41"/>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B20" s="39"/>
       <c r="C20" s="41"/>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B21" s="39"/>
       <c r="C21" s="41"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B22" s="39"/>
       <c r="C22" s="41"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B23" s="39"/>
       <c r="C23" s="41"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B24" s="39"/>
       <c r="C24" s="41"/>
     </row>
-    <row r="25" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B25" s="39"/>
       <c r="C25" s="41"/>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B26" s="39"/>
       <c r="C26" s="41"/>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B27" s="39"/>
       <c r="C27" s="41"/>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B28" s="39"/>
       <c r="C28" s="41"/>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B29" s="39"/>
       <c r="C29" s="41"/>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B30" s="39"/>
       <c r="C30" s="41"/>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B31" s="39"/>
       <c r="C31" s="41"/>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B32" s="39"/>
       <c r="C32" s="41"/>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B33" s="39"/>
       <c r="C33" s="41"/>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B34" s="39"/>
       <c r="C34" s="41"/>
     </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B35" s="39"/>
       <c r="C35" s="41"/>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B36" s="39"/>
       <c r="C36" s="41"/>
     </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B37" s="39"/>
       <c r="C37" s="41"/>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B38" s="39"/>
       <c r="C38" s="41"/>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B39" s="39"/>
       <c r="C39" s="41"/>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B40" s="39"/>
       <c r="C40" s="41"/>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B41" s="39"/>
       <c r="C41" s="41"/>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B42" s="39"/>
       <c r="C42" s="41"/>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B43" s="39"/>
       <c r="C43" s="41"/>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B44" s="40"/>
       <c r="C44" s="41"/>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B45" s="40"/>
       <c r="C45" s="41"/>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B46" s="40"/>
       <c r="C46" s="41"/>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B47" s="40"/>
       <c r="C47" s="41"/>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B48" s="39"/>
       <c r="C48" s="41"/>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="39"/>
       <c r="C49" s="41"/>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="39"/>
       <c r="C50" s="41"/>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="39"/>
       <c r="C51" s="41"/>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="39"/>
       <c r="C52" s="41"/>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="39"/>
       <c r="C53" s="41"/>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="39"/>
       <c r="C54" s="41"/>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="39"/>
       <c r="C55" s="41"/>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="39"/>
       <c r="C56" s="41"/>
     </row>
@@ -3430,16 +3450,16 @@
       <selection pane="bottomRight" activeCell="A38" sqref="A38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.41796875" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="35" customWidth="1"/>
-    <col min="2" max="2" width="32.68359375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.83984375" customWidth="1"/>
-    <col min="6" max="6" width="52.26171875" bestFit="1" customWidth="1"/>
-    <col min="81" max="86" width="11.578125" style="12"/>
+    <col min="2" max="2" width="32.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" customWidth="1"/>
+    <col min="6" max="6" width="52.28515625" bestFit="1" customWidth="1"/>
+    <col min="81" max="86" width="11.5703125" style="12"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:277" ht="17.7" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:277" ht="18" x14ac:dyDescent="0.25">
       <c r="A1" s="19" t="s">
         <v>48</v>
       </c>
@@ -3725,7 +3745,7 @@
       <c r="JP1" s="2"/>
       <c r="JQ1" s="2"/>
     </row>
-    <row r="2" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>51</v>
       </c>
@@ -4011,7 +4031,7 @@
       <c r="JP2" s="2"/>
       <c r="JQ2" s="2"/>
     </row>
-    <row r="3" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>50</v>
       </c>
@@ -4297,7 +4317,7 @@
       <c r="JP3" s="2"/>
       <c r="JQ3" s="2"/>
     </row>
-    <row r="4" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>55</v>
       </c>
@@ -4583,7 +4603,7 @@
       <c r="JP4" s="2"/>
       <c r="JQ4" s="2"/>
     </row>
-    <row r="5" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B5" s="30"/>
       <c r="C5" t="s">
         <v>53</v>
@@ -4861,7 +4881,7 @@
       <c r="JP5" s="2"/>
       <c r="JQ5" s="2"/>
     </row>
-    <row r="6" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>58</v>
       </c>
@@ -5142,7 +5162,7 @@
       <c r="JP6" s="2"/>
       <c r="JQ6" s="2"/>
     </row>
-    <row r="7" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>59</v>
       </c>
@@ -5428,7 +5448,7 @@
       <c r="JP7" s="2"/>
       <c r="JQ7" s="2"/>
     </row>
-    <row r="8" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>61</v>
       </c>
@@ -5714,7 +5734,7 @@
       <c r="JP8" s="2"/>
       <c r="JQ8" s="2"/>
     </row>
-    <row r="9" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>63</v>
       </c>
@@ -6000,7 +6020,7 @@
       <c r="JP9" s="2"/>
       <c r="JQ9" s="2"/>
     </row>
-    <row r="10" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>65</v>
       </c>
@@ -6286,7 +6306,7 @@
       <c r="JP10" s="2"/>
       <c r="JQ10" s="2"/>
     </row>
-    <row r="11" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>67</v>
       </c>
@@ -6572,7 +6592,7 @@
       <c r="JP11" s="2"/>
       <c r="JQ11" s="2"/>
     </row>
-    <row r="12" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>50</v>
       </c>
@@ -6861,7 +6881,7 @@
       <c r="JP12" s="2"/>
       <c r="JQ12" s="2"/>
     </row>
-    <row r="13" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>55</v>
       </c>
@@ -7147,7 +7167,7 @@
       <c r="JP13" s="2"/>
       <c r="JQ13" s="2"/>
     </row>
-    <row r="14" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>74</v>
       </c>
@@ -7433,7 +7453,7 @@
       <c r="JP14" s="2"/>
       <c r="JQ14" s="2"/>
     </row>
-    <row r="15" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B15" s="30"/>
       <c r="C15" t="s">
         <v>53</v>
@@ -7711,7 +7731,7 @@
       <c r="JP15" s="2"/>
       <c r="JQ15" s="2"/>
     </row>
-    <row r="16" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:277" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>53</v>
       </c>
@@ -7987,7 +8007,7 @@
       <c r="JP16" s="2"/>
       <c r="JQ16" s="2"/>
     </row>
-    <row r="17" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -8272,7 +8292,7 @@
       <c r="JP17" s="2"/>
       <c r="JQ17" s="2"/>
     </row>
-    <row r="18" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>76</v>
       </c>
@@ -8558,7 +8578,7 @@
       <c r="JP18" s="2"/>
       <c r="JQ18" s="2"/>
     </row>
-    <row r="19" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>59</v>
       </c>
@@ -8844,7 +8864,7 @@
       <c r="JP19" s="2"/>
       <c r="JQ19" s="2"/>
     </row>
-    <row r="20" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>50</v>
       </c>
@@ -9130,7 +9150,7 @@
       <c r="JP20" s="2"/>
       <c r="JQ20" s="2"/>
     </row>
-    <row r="21" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>51</v>
       </c>
@@ -9416,7 +9436,7 @@
       <c r="JP21" s="2"/>
       <c r="JQ21" s="2"/>
     </row>
-    <row r="22" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>65</v>
       </c>
@@ -9702,7 +9722,7 @@
       <c r="JP22" s="2"/>
       <c r="JQ22" s="2"/>
     </row>
-    <row r="23" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>67</v>
       </c>
@@ -9988,7 +10008,7 @@
       <c r="JP23" s="2"/>
       <c r="JQ23" s="2"/>
     </row>
-    <row r="24" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:277" x14ac:dyDescent="0.25">
       <c r="E24" s="2"/>
       <c r="G24" s="9"/>
       <c r="H24" s="9"/>
@@ -10262,7 +10282,7 @@
       <c r="JP24" s="2"/>
       <c r="JQ24" s="2"/>
     </row>
-    <row r="25" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>61</v>
       </c>
@@ -10548,7 +10568,7 @@
       <c r="JP25" s="2"/>
       <c r="JQ25" s="2"/>
     </row>
-    <row r="26" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:277" x14ac:dyDescent="0.25">
       <c r="E26" s="2"/>
       <c r="G26" s="9"/>
       <c r="H26" s="9"/>
@@ -10822,7 +10842,7 @@
       <c r="JP26" s="2"/>
       <c r="JQ26" s="2"/>
     </row>
-    <row r="27" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>81</v>
       </c>
@@ -11110,7 +11130,7 @@
       <c r="JP27" s="2"/>
       <c r="JQ27" s="2"/>
     </row>
-    <row r="28" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>50</v>
       </c>
@@ -11396,7 +11416,7 @@
       <c r="JP28" s="2"/>
       <c r="JQ28" s="2"/>
     </row>
-    <row r="29" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>82</v>
       </c>
@@ -11683,7 +11703,7 @@
       <c r="JP29" s="2"/>
       <c r="JQ29" s="2"/>
     </row>
-    <row r="30" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>84</v>
       </c>
@@ -11969,7 +11989,7 @@
       <c r="JP30" s="2"/>
       <c r="JQ30" s="2"/>
     </row>
-    <row r="31" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>59</v>
       </c>
@@ -12252,7 +12272,7 @@
       <c r="JP31" s="2"/>
       <c r="JQ31" s="2"/>
     </row>
-    <row r="32" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>85</v>
       </c>
@@ -12536,7 +12556,7 @@
       <c r="JP32" s="2"/>
       <c r="JQ32" s="2"/>
     </row>
-    <row r="33" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>97</v>
       </c>
@@ -12822,7 +12842,7 @@
       <c r="JP33" s="2"/>
       <c r="JQ33" s="2"/>
     </row>
-    <row r="34" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>98</v>
       </c>
@@ -13108,7 +13128,7 @@
       <c r="JP34" s="2"/>
       <c r="JQ34" s="2"/>
     </row>
-    <row r="35" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>99</v>
       </c>
@@ -13394,7 +13414,7 @@
       <c r="JP35" s="2"/>
       <c r="JQ35" s="2"/>
     </row>
-    <row r="36" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>67</v>
       </c>
@@ -13680,7 +13700,7 @@
       <c r="JP36" s="2"/>
       <c r="JQ36" s="2"/>
     </row>
-    <row r="37" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>101</v>
       </c>
@@ -13966,7 +13986,7 @@
       <c r="JP37" s="2"/>
       <c r="JQ37" s="2"/>
     </row>
-    <row r="38" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>51</v>
       </c>
@@ -14252,7 +14272,7 @@
       <c r="JP38" s="2"/>
       <c r="JQ38" s="2"/>
     </row>
-    <row r="39" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:277" x14ac:dyDescent="0.25">
       <c r="F39" s="2"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
@@ -14526,7 +14546,7 @@
       <c r="JP39" s="2"/>
       <c r="JQ39" s="2"/>
     </row>
-    <row r="40" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -14812,7 +14832,7 @@
       <c r="JP40" s="2"/>
       <c r="JQ40" s="2"/>
     </row>
-    <row r="41" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B41" s="30"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
@@ -15087,7 +15107,7 @@
       <c r="JP41" s="2"/>
       <c r="JQ41" s="2"/>
     </row>
-    <row r="42" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B42" s="30"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
@@ -15362,7 +15382,7 @@
       <c r="JP42" s="2"/>
       <c r="JQ42" s="2"/>
     </row>
-    <row r="43" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B43" s="30"/>
       <c r="F43" s="2"/>
       <c r="G43" s="2"/>
@@ -15637,7 +15657,7 @@
       <c r="JP43" s="2"/>
       <c r="JQ43" s="2"/>
     </row>
-    <row r="44" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -15923,7 +15943,7 @@
       <c r="JP44" s="2"/>
       <c r="JQ44" s="2"/>
     </row>
-    <row r="45" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>104</v>
       </c>
@@ -16209,7 +16229,7 @@
       <c r="JP45" s="2"/>
       <c r="JQ45" s="2"/>
     </row>
-    <row r="46" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>105</v>
       </c>
@@ -16495,7 +16515,7 @@
       <c r="JP46" s="2"/>
       <c r="JQ46" s="2"/>
     </row>
-    <row r="47" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>87</v>
       </c>
@@ -16781,7 +16801,7 @@
       <c r="JP47" s="2"/>
       <c r="JQ47" s="2"/>
     </row>
-    <row r="48" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>81</v>
       </c>
@@ -17067,7 +17087,7 @@
       <c r="JP48" s="2"/>
       <c r="JQ48" s="2"/>
     </row>
-    <row r="49" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>88</v>
       </c>
@@ -17353,7 +17373,7 @@
       <c r="JP49" s="2"/>
       <c r="JQ49" s="2"/>
     </row>
-    <row r="50" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>89</v>
       </c>
@@ -17639,7 +17659,7 @@
       <c r="JP50" s="2"/>
       <c r="JQ50" s="2"/>
     </row>
-    <row r="51" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>91</v>
       </c>
@@ -17925,7 +17945,7 @@
       <c r="JP51" s="2"/>
       <c r="JQ51" s="2"/>
     </row>
-    <row r="52" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>106</v>
       </c>
@@ -18208,7 +18228,7 @@
       <c r="JP52" s="2"/>
       <c r="JQ52" s="2"/>
     </row>
-    <row r="53" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B53" s="30"/>
       <c r="F53" s="2"/>
       <c r="G53" s="2"/>
@@ -18483,7 +18503,7 @@
       <c r="JP53" s="2"/>
       <c r="JQ53" s="2"/>
     </row>
-    <row r="54" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:277" x14ac:dyDescent="0.25">
       <c r="B54" s="30"/>
       <c r="F54" s="2"/>
       <c r="G54" s="2"/>
@@ -18758,7 +18778,7 @@
       <c r="JP54" s="2"/>
       <c r="JQ54" s="2"/>
     </row>
-    <row r="55" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>107</v>
       </c>
@@ -18778,7 +18798,7 @@
       <c r="CL55" s="12"/>
       <c r="CP55" s="12"/>
     </row>
-    <row r="56" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>108</v>
       </c>
@@ -18798,7 +18818,7 @@
       <c r="CL56" s="12"/>
       <c r="CP56" s="12"/>
     </row>
-    <row r="57" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>109</v>
       </c>
@@ -18818,7 +18838,7 @@
       <c r="CL57" s="12"/>
       <c r="CP57" s="12"/>
     </row>
-    <row r="58" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>110</v>
       </c>
@@ -18838,7 +18858,7 @@
       <c r="CL58" s="12"/>
       <c r="CP58" s="12"/>
     </row>
-    <row r="59" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>111</v>
       </c>
@@ -18858,7 +18878,7 @@
       <c r="CL59" s="12"/>
       <c r="CP59" s="12"/>
     </row>
-    <row r="60" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:277" x14ac:dyDescent="0.25">
       <c r="G60" s="30"/>
       <c r="CI60" s="12"/>
       <c r="CJ60" s="12"/>
@@ -18866,7 +18886,7 @@
       <c r="CL60" s="12"/>
       <c r="CP60" s="12"/>
     </row>
-    <row r="61" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:277" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>113</v>
       </c>
@@ -18880,7 +18900,7 @@
       <c r="CL61" s="12"/>
       <c r="CP61" s="12"/>
     </row>
-    <row r="62" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:277" x14ac:dyDescent="0.25">
       <c r="G62" s="30"/>
       <c r="CI62" s="12"/>
       <c r="CJ62" s="12"/>
@@ -18888,7 +18908,7 @@
       <c r="CL62" s="12"/>
       <c r="CP62" s="12"/>
     </row>
-    <row r="63" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:277" x14ac:dyDescent="0.25">
       <c r="G63" s="30"/>
       <c r="CI63" s="12"/>
       <c r="CJ63" s="12"/>
@@ -18896,7 +18916,7 @@
       <c r="CL63" s="12"/>
       <c r="CP63" s="12"/>
     </row>
-    <row r="64" spans="1:277" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:277" x14ac:dyDescent="0.25">
       <c r="G64" s="30"/>
       <c r="CI64" s="12"/>
       <c r="CJ64" s="12"/>
@@ -18904,34 +18924,34 @@
       <c r="CL64" s="12"/>
       <c r="CP64" s="12"/>
     </row>
-    <row r="65" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G65" s="30"/>
     </row>
-    <row r="66" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G66" s="30"/>
     </row>
-    <row r="67" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G67" s="30"/>
     </row>
-    <row r="68" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G68" s="30"/>
     </row>
-    <row r="69" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G69" s="30"/>
     </row>
-    <row r="70" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G70" s="30"/>
     </row>
-    <row r="71" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G71" s="30"/>
     </row>
-    <row r="72" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G72" s="30"/>
     </row>
-    <row r="73" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G73" s="30"/>
     </row>
-    <row r="74" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G74" s="30"/>
       <c r="BW74" s="12"/>
       <c r="BX74" s="12"/>
@@ -18940,7 +18960,7 @@
       <c r="CA74" s="12"/>
       <c r="CB74" s="12"/>
     </row>
-    <row r="75" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G75" s="30"/>
       <c r="BW75" s="12"/>
       <c r="BX75" s="12"/>
@@ -18949,7 +18969,7 @@
       <c r="CA75" s="12"/>
       <c r="CB75" s="12"/>
     </row>
-    <row r="76" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G76" s="30"/>
       <c r="BW76" s="12"/>
       <c r="BX76" s="12"/>
@@ -18958,7 +18978,7 @@
       <c r="CA76" s="12"/>
       <c r="CB76" s="12"/>
     </row>
-    <row r="77" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G77" s="30"/>
       <c r="BW77" s="12"/>
       <c r="BX77" s="12"/>
@@ -18967,7 +18987,7 @@
       <c r="CA77" s="12"/>
       <c r="CB77" s="12"/>
     </row>
-    <row r="78" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="3:87" x14ac:dyDescent="0.25">
       <c r="C78" s="23"/>
       <c r="G78" s="30"/>
       <c r="BW78" s="12"/>
@@ -18977,7 +18997,7 @@
       <c r="CA78" s="12"/>
       <c r="CB78" s="12"/>
     </row>
-    <row r="79" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="3:87" x14ac:dyDescent="0.25">
       <c r="G79" s="30"/>
       <c r="BW79" s="12"/>
       <c r="BX79" s="12"/>
@@ -18987,7 +19007,7 @@
       <c r="CB79" s="12"/>
       <c r="CI79" s="25"/>
     </row>
-    <row r="80" spans="3:87" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="3:87" x14ac:dyDescent="0.25">
       <c r="BW80" s="12"/>
       <c r="BX80" s="12"/>
       <c r="BY80" s="12"/>
@@ -18996,7 +19016,7 @@
       <c r="CB80" s="12"/>
       <c r="CI80" s="26"/>
     </row>
-    <row r="81" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A81" s="20"/>
       <c r="BW81" s="12"/>
       <c r="BX81" s="12"/>
@@ -19007,7 +19027,7 @@
       <c r="CI81" s="25"/>
       <c r="CJ81" s="25"/>
     </row>
-    <row r="82" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A82" s="20"/>
       <c r="BW82" s="12"/>
       <c r="BX82" s="12"/>
@@ -19018,7 +19038,7 @@
       <c r="CI82" s="25"/>
       <c r="CJ82" s="25"/>
     </row>
-    <row r="83" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A83" s="20"/>
       <c r="BW83" s="12"/>
       <c r="BX83" s="12"/>
@@ -19029,7 +19049,7 @@
       <c r="CI83" s="25"/>
       <c r="CJ83" s="26"/>
     </row>
-    <row r="84" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A84" s="20"/>
       <c r="BW84" s="12"/>
       <c r="BX84" s="12"/>
@@ -19041,7 +19061,7 @@
       <c r="CJ84" s="25"/>
       <c r="CL84" s="25"/>
     </row>
-    <row r="85" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A85" s="20"/>
       <c r="BW85" s="12"/>
       <c r="BX85" s="12"/>
@@ -19055,7 +19075,7 @@
       <c r="CL85" s="25"/>
       <c r="CP85" s="25"/>
     </row>
-    <row r="86" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A86" s="20"/>
       <c r="BW86" s="12"/>
       <c r="BX86" s="12"/>
@@ -19069,7 +19089,7 @@
       <c r="CL86" s="25"/>
       <c r="CP86" s="25"/>
     </row>
-    <row r="87" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A87" s="20"/>
       <c r="BW87" s="12"/>
       <c r="BX87" s="12"/>
@@ -19083,7 +19103,7 @@
       <c r="CL87" s="25"/>
       <c r="CP87" s="25"/>
     </row>
-    <row r="88" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A88" s="20"/>
       <c r="BW88" s="12"/>
       <c r="BX88" s="12"/>
@@ -19097,7 +19117,7 @@
       <c r="CL88" s="25"/>
       <c r="CP88" s="25"/>
     </row>
-    <row r="89" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A89" s="20"/>
       <c r="BW89" s="12"/>
       <c r="BX89" s="12"/>
@@ -19111,7 +19131,7 @@
       <c r="CL89" s="25"/>
       <c r="CP89" s="25"/>
     </row>
-    <row r="90" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A90" s="20"/>
       <c r="BW90" s="12"/>
       <c r="BX90" s="12"/>
@@ -19125,7 +19145,7 @@
       <c r="CL90" s="25"/>
       <c r="CP90" s="25"/>
     </row>
-    <row r="91" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A91" s="20"/>
       <c r="BW91" s="12"/>
       <c r="BX91" s="12"/>
@@ -19139,7 +19159,7 @@
       <c r="CL91" s="26"/>
       <c r="CP91" s="25"/>
     </row>
-    <row r="92" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A92" s="20"/>
       <c r="BW92" s="12"/>
       <c r="BX92" s="12"/>
@@ -19153,7 +19173,7 @@
       <c r="CL92" s="25"/>
       <c r="CP92" s="25"/>
     </row>
-    <row r="93" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A93" s="20"/>
       <c r="BW93" s="12"/>
       <c r="BX93" s="12"/>
@@ -19167,7 +19187,7 @@
       <c r="CL93" s="25"/>
       <c r="CP93" s="25"/>
     </row>
-    <row r="94" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A94" s="20"/>
       <c r="BW94" s="12"/>
       <c r="BX94" s="12"/>
@@ -19181,7 +19201,7 @@
       <c r="CL94" s="25"/>
       <c r="CP94" s="25"/>
     </row>
-    <row r="95" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A95" s="20"/>
       <c r="BW95" s="12"/>
       <c r="BX95" s="12"/>
@@ -19195,7 +19215,7 @@
       <c r="CL95" s="25"/>
       <c r="CP95" s="25"/>
     </row>
-    <row r="96" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A96" s="20"/>
       <c r="BW96" s="12"/>
       <c r="BX96" s="12"/>
@@ -19209,7 +19229,7 @@
       <c r="CL96" s="25"/>
       <c r="CP96" s="25"/>
     </row>
-    <row r="97" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A97" s="20"/>
       <c r="BW97" s="12"/>
       <c r="BX97" s="12"/>
@@ -19223,7 +19243,7 @@
       <c r="CL97" s="25"/>
       <c r="CP97" s="26"/>
     </row>
-    <row r="98" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A98" s="20"/>
       <c r="BW98" s="12"/>
       <c r="BX98" s="12"/>
@@ -19237,7 +19257,7 @@
       <c r="CL98" s="25"/>
       <c r="CP98" s="26"/>
     </row>
-    <row r="99" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A99" s="20"/>
       <c r="BW99" s="12"/>
       <c r="BX99" s="12"/>
@@ -19251,7 +19271,7 @@
       <c r="CL99" s="28"/>
       <c r="CP99" s="25"/>
     </row>
-    <row r="100" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A100" s="20"/>
       <c r="BW100" s="12"/>
       <c r="BX100" s="12"/>
@@ -19266,7 +19286,7 @@
       <c r="CL100" s="25"/>
       <c r="CP100" s="25"/>
     </row>
-    <row r="101" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A101" s="20"/>
       <c r="BW101" s="12"/>
       <c r="BX101" s="12"/>
@@ -19281,7 +19301,7 @@
       <c r="CL101" s="25"/>
       <c r="CP101" s="25"/>
     </row>
-    <row r="102" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A102" s="20"/>
       <c r="BW102" s="12"/>
       <c r="BX102" s="12"/>
@@ -19296,7 +19316,7 @@
       <c r="CL102" s="25"/>
       <c r="CP102" s="25"/>
     </row>
-    <row r="103" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A103" s="20"/>
       <c r="BW103" s="12"/>
       <c r="BX103" s="12"/>
@@ -19311,7 +19331,7 @@
       <c r="CL103" s="25"/>
       <c r="CP103" s="25"/>
     </row>
-    <row r="104" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A104" s="20"/>
       <c r="BW104" s="12"/>
       <c r="BX104" s="12"/>
@@ -19326,7 +19346,7 @@
       <c r="CL104" s="25"/>
       <c r="CP104" s="25"/>
     </row>
-    <row r="105" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A105" s="20"/>
       <c r="BW105" s="12"/>
       <c r="BX105" s="12"/>
@@ -19341,7 +19361,7 @@
       <c r="CL105" s="25"/>
       <c r="CP105" s="25"/>
     </row>
-    <row r="106" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A106" s="20"/>
       <c r="BW106" s="12"/>
       <c r="BX106" s="12"/>
@@ -19356,7 +19376,7 @@
       <c r="CL106" s="25"/>
       <c r="CP106" s="25"/>
     </row>
-    <row r="107" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A107" s="20"/>
       <c r="BW107" s="12"/>
       <c r="BX107" s="12"/>
@@ -19371,7 +19391,7 @@
       <c r="CL107" s="25"/>
       <c r="CP107" s="25"/>
     </row>
-    <row r="108" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A108" s="20"/>
       <c r="BW108" s="12"/>
       <c r="BX108" s="12"/>
@@ -19386,7 +19406,7 @@
       <c r="CL108" s="25"/>
       <c r="CP108" s="25"/>
     </row>
-    <row r="109" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A109" s="20"/>
       <c r="BW109" s="12"/>
       <c r="BX109" s="12"/>
@@ -19401,7 +19421,7 @@
       <c r="CL109" s="25"/>
       <c r="CP109" s="25"/>
     </row>
-    <row r="110" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A110" s="20"/>
       <c r="E110" s="23"/>
       <c r="F110" s="23"/>
@@ -19419,7 +19439,7 @@
       <c r="CL110" s="25"/>
       <c r="CP110" s="25"/>
     </row>
-    <row r="111" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A111" s="20"/>
       <c r="BW111" s="12"/>
       <c r="BX111" s="12"/>
@@ -19428,7 +19448,7 @@
       <c r="CA111" s="12"/>
       <c r="CB111" s="12"/>
     </row>
-    <row r="112" spans="1:94" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:94" x14ac:dyDescent="0.25">
       <c r="A112" s="20"/>
       <c r="BW112" s="12"/>
       <c r="BX112" s="12"/>
@@ -19437,261 +19457,261 @@
       <c r="CA112" s="12"/>
       <c r="CB112" s="12"/>
     </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" s="20"/>
     </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" s="20"/>
     </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" s="20"/>
     </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" s="20"/>
     </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" s="20"/>
     </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" s="20"/>
     </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" s="20"/>
     </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" s="20"/>
     </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" s="20"/>
     </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="20"/>
     </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" s="20"/>
       <c r="B123" s="2"/>
     </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" s="20"/>
       <c r="B124" s="2"/>
     </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" s="20"/>
       <c r="B125" s="2"/>
     </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" s="20"/>
       <c r="B126" s="2"/>
     </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" s="20"/>
       <c r="B127" s="2"/>
     </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" s="20"/>
       <c r="B128" s="2"/>
     </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" s="20"/>
       <c r="B129" s="2"/>
     </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" s="20"/>
       <c r="B130" s="2"/>
     </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" s="20"/>
       <c r="B131" s="2"/>
     </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" s="20"/>
       <c r="B132" s="2"/>
     </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" s="20"/>
       <c r="B133" s="2"/>
     </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" s="20"/>
       <c r="B134" s="2"/>
     </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" s="20"/>
       <c r="B135" s="2"/>
     </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" s="20"/>
       <c r="B136" s="2"/>
     </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" s="20"/>
       <c r="B137" s="2"/>
     </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" s="20"/>
       <c r="B138" s="2"/>
     </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" s="20"/>
       <c r="B139" s="2"/>
     </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" s="20"/>
       <c r="B140" s="2"/>
     </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" s="20"/>
       <c r="B141" s="2"/>
     </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" s="20"/>
       <c r="B142" s="2"/>
     </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" s="20"/>
       <c r="B143" s="2"/>
     </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" s="20"/>
       <c r="B144" s="2"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" s="20"/>
       <c r="B145" s="2"/>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" s="20"/>
       <c r="B146" s="2"/>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" s="20"/>
       <c r="B147" s="2"/>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" s="20"/>
       <c r="B148" s="2"/>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" s="20"/>
       <c r="B149" s="2"/>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" s="20"/>
       <c r="B150" s="2"/>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" s="20"/>
       <c r="B151" s="2"/>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" s="20"/>
       <c r="B152" s="2"/>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" s="20"/>
       <c r="B153" s="2"/>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" s="20"/>
       <c r="B154" s="2"/>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" s="20"/>
       <c r="B155" s="2"/>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" s="20"/>
       <c r="B156" s="2"/>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" s="20"/>
       <c r="B157" s="2"/>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" s="20"/>
       <c r="B158" s="2"/>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" s="20"/>
       <c r="B159" s="2"/>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" s="20"/>
       <c r="B160" s="2"/>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" s="20"/>
       <c r="B161" s="2"/>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" s="20"/>
       <c r="B162" s="2"/>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" s="20"/>
       <c r="B163" s="2"/>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" s="20"/>
       <c r="B164" s="2"/>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" s="20"/>
       <c r="B165" s="2"/>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" s="20"/>
       <c r="B166" s="2"/>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" s="20"/>
       <c r="B167" s="2"/>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" s="20"/>
       <c r="B168" s="2"/>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" s="20"/>
       <c r="B169" s="2"/>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" s="20"/>
       <c r="B170" s="2"/>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" s="20"/>
       <c r="B171" s="2"/>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="20"/>
       <c r="B172" s="2"/>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" s="20"/>
       <c r="B173" s="2"/>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" s="20"/>
       <c r="B174" s="2"/>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" s="20"/>
       <c r="B175" s="2"/>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" s="20"/>
       <c r="B176" s="2"/>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" s="20"/>
       <c r="B177" s="2"/>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" s="20"/>
       <c r="B178" s="2"/>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" s="20"/>
       <c r="B179" s="2"/>
     </row>
@@ -19717,19 +19737,19 @@
       <selection activeCell="B7" sqref="B7:B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="50.83984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83984375" customWidth="1"/>
-    <col min="3" max="3" width="18.83984375" style="35" customWidth="1"/>
-    <col min="4" max="4" width="16.578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="50.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="35" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.83984375" customWidth="1"/>
-    <col min="8" max="8" width="12.26171875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.85546875" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>115</v>
       </c>
@@ -19743,7 +19763,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>79</v>
       </c>
@@ -19757,7 +19777,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -19771,7 +19791,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>117</v>
       </c>
@@ -19785,7 +19805,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>118</v>
       </c>
@@ -19799,7 +19819,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>119</v>
       </c>
@@ -19813,7 +19833,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>120</v>
       </c>
@@ -19827,7 +19847,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>121</v>
       </c>
@@ -19841,7 +19861,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>122</v>
       </c>
@@ -19855,35 +19875,35 @@
         <v>123</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
       <c r="B11" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>189</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A12" t="s">
-        <v>190</v>
       </c>
       <c r="B12">
         <v>0.9</v>
       </c>
       <c r="D12" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B13">
         <v>1.996</v>
       </c>
       <c r="D13" t="s">
-        <v>192</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="46"/>
       <c r="B14" s="46"/>
       <c r="C14" s="46"/>
@@ -19894,37 +19914,37 @@
       <c r="H14" s="46"/>
       <c r="I14" s="46"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="45"/>
       <c r="B15" s="45" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C15" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>198</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>192</v>
+      </c>
+      <c r="F15" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="50" t="s">
+        <v>196</v>
+      </c>
+      <c r="H15" s="50" t="s">
+        <v>195</v>
+      </c>
+      <c r="J15" s="50" t="s">
         <v>200</v>
       </c>
-      <c r="D15" s="45" t="s">
-        <v>199</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="F15" s="45" t="s">
+      <c r="K15" s="49"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>189</v>
-      </c>
-      <c r="G15" s="50" t="s">
-        <v>197</v>
-      </c>
-      <c r="H15" s="50" t="s">
-        <v>196</v>
-      </c>
-      <c r="J15" s="50" t="s">
-        <v>201</v>
-      </c>
-      <c r="K15" s="49"/>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
-      <c r="A16" t="s">
-        <v>190</v>
       </c>
       <c r="B16">
         <v>9</v>
@@ -19947,9 +19967,9 @@
         <v>4.05</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D17" s="35">
         <v>2</v>
@@ -19969,9 +19989,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="44" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B18" s="44">
         <f>SUM(B16:B17)</f>
@@ -19996,16 +20016,16 @@
         <v>51.851851851851855</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B21">
         <f>1000/H18</f>
         <v>246.9135802469136</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B22">
         <f>B21*J16</f>
         <v>0</v>
@@ -20016,4 +20036,608 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBC3B418-F353-48F3-81CC-971E8DA13285}">
+  <dimension ref="B1:C127"/>
+  <sheetViews>
+    <sheetView topLeftCell="A100" workbookViewId="0">
+      <selection activeCell="A100" sqref="A1:B1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" style="35" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="C1" s="2" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="35"/>
+      <c r="C2" s="35" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="35"/>
+      <c r="C3" s="35" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B4" s="35"/>
+      <c r="C4" s="35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B5" s="35"/>
+      <c r="C5" s="35" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B8" s="35"/>
+      <c r="C8" s="35" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B9" s="35"/>
+      <c r="C9" s="35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B10" s="35"/>
+      <c r="C10" s="35" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B12" s="35"/>
+      <c r="C12" s="35" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" s="35"/>
+      <c r="C13" s="35" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="14" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B14" s="35"/>
+      <c r="C14" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B15" s="35"/>
+      <c r="C15" s="35" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B17" s="35"/>
+      <c r="C17" s="38" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B18" s="35"/>
+      <c r="C18" s="38" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B19" s="35"/>
+      <c r="C19" s="38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B20" s="35"/>
+      <c r="C20" s="35" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B21" s="35"/>
+      <c r="C21" s="35" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B22" s="35"/>
+      <c r="C22" s="35" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="23" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B23" s="35"/>
+      <c r="C23" s="35" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B24" s="35"/>
+      <c r="C24" s="35" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="25" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B25" s="35"/>
+      <c r="C25" s="35" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="26" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B26" s="35"/>
+      <c r="C26" s="35" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="27" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B27" s="35"/>
+      <c r="C27" s="35" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="28" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B28" s="35"/>
+      <c r="C28" s="35" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="29" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="35"/>
+      <c r="C29" s="35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="30" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B30" s="35"/>
+      <c r="C30" s="35" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="31" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B31" s="35"/>
+      <c r="C31" s="35" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B32" s="35"/>
+      <c r="C32" s="35" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B33" s="35"/>
+      <c r="C33" s="35" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B34" s="35"/>
+      <c r="C34" s="35" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B35" s="35"/>
+      <c r="C35" s="35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B36" s="35"/>
+      <c r="C36" s="35" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B37" s="35"/>
+      <c r="C37" s="35" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B38" s="35"/>
+      <c r="C38" s="35" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B39" s="35"/>
+      <c r="C39" s="35" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B40" s="35"/>
+      <c r="C40" s="35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B41" s="35"/>
+      <c r="C41" s="35" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B42" s="35"/>
+      <c r="C42" s="35" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B43" s="35"/>
+      <c r="C43" s="35" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B44" s="35"/>
+      <c r="C44" s="35" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B45" s="35"/>
+      <c r="C45" s="35" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B46" s="35"/>
+      <c r="C46" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="35"/>
+      <c r="C47" s="35" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B48" s="35"/>
+      <c r="C48" s="35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B49" s="35"/>
+      <c r="C49" s="35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B50" s="35"/>
+      <c r="C50" s="35" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B51" s="35"/>
+      <c r="C51" s="35" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B52" s="35"/>
+      <c r="C52" s="35" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B53" s="35"/>
+      <c r="C53" s="35" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B54" s="35"/>
+      <c r="C54" s="35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B55" s="35"/>
+      <c r="C55" s="35" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B56" s="35"/>
+      <c r="C56" s="35" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B57" s="35"/>
+      <c r="C57" s="35" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B58" s="35"/>
+      <c r="C58" s="35" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B59" s="35"/>
+      <c r="C59" s="35" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B60" s="35"/>
+      <c r="C60" s="35" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B61" s="35"/>
+      <c r="C61" s="35" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B62" s="35"/>
+      <c r="C62" s="35" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B63" s="35"/>
+      <c r="C63" s="35" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B64" s="35"/>
+      <c r="C64" s="35" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="35"/>
+      <c r="C65" s="35" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B66" s="35"/>
+      <c r="C66" s="35" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B67" s="35"/>
+      <c r="C67" s="35" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B68" s="35"/>
+      <c r="C68" s="51"/>
+    </row>
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B69" s="35"/>
+      <c r="C69" s="51"/>
+    </row>
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B70" s="35"/>
+    </row>
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B71" s="35"/>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B72" s="35"/>
+    </row>
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B73" s="35"/>
+    </row>
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B74" s="35"/>
+    </row>
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B75" s="35"/>
+    </row>
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B76" s="35"/>
+    </row>
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B77" s="35"/>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B78" s="35"/>
+    </row>
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B79" s="35"/>
+    </row>
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B80" s="35"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="35"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="35"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="35"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="35"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" s="35"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" s="35"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" s="35"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" s="35"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" s="35"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="35"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="35"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" s="35"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" s="35"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" s="35"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" s="35"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" s="35"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B97" s="35"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B98" s="35"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="35"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B100" s="35"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B101" s="35"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B102" s="35"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B103" s="35"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B104" s="35"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B105" s="35"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B106" s="35"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B107" s="35"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B108" s="35"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B109" s="35"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B110" s="35"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B111" s="35"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B112" s="35"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" s="35"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" s="35"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" s="35"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" s="35"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" s="35"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B118" s="35"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B119" s="35"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" s="35"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" s="35"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" s="35"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" s="35"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" s="35"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" s="35"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" s="35"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" s="35"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>